<commit_message>
Updated to Version 1.2
Added Priority and Test Scenarios IDs
</commit_message>
<xml_diff>
--- a/test_cases/TC-03.xlsx
+++ b/test_cases/TC-03.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="94">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -82,6 +82,9 @@
     <t>Pass = !23reTeAf</t>
   </si>
   <si>
+    <t>New_Pass = 65&amp;uTper</t>
+  </si>
+  <si>
     <t>DoB = 03/02/1992</t>
   </si>
   <si>
@@ -97,10 +100,22 @@
     <t>State = Houston</t>
   </si>
   <si>
-    <t>Postal Code = 1234</t>
-  </si>
-  <si>
-    <t>Phone = +48512354</t>
+    <t>Zip Code = 10017</t>
+  </si>
+  <si>
+    <t>Phone = +148512354</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>TS-3A</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
   <si>
     <t>Test Scenario</t>
@@ -250,6 +265,9 @@
     <t>DF-001: Site did not open</t>
   </si>
   <si>
+    <t>TS-3B</t>
+  </si>
+  <si>
     <t>Alternate Test Scenario 1</t>
   </si>
   <si>
@@ -263,6 +281,9 @@
   </si>
   <si>
     <t>DF-012: User was allowed to input same password and account was updated</t>
+  </si>
+  <si>
+    <t>TS-3C</t>
   </si>
   <si>
     <t>Alternate Test Scenario 2</t>
@@ -371,7 +392,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +403,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
     <fill>
@@ -605,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -676,6 +703,24 @@
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="11" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -689,7 +734,7 @@
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="17" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -706,10 +751,10 @@
     <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="17" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -721,7 +766,7 @@
     <xf borderId="9" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="20" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="20" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -744,6 +789,9 @@
     </xf>
     <xf borderId="9" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1020,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="13">
-        <v>44562.0</v>
+        <v>44593.0</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -1138,15 +1186,15 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="D12" s="23">
-        <v>5.0</v>
-      </c>
-      <c r="E12" s="24" t="s">
+        <v>4.0</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="D13" s="23">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="E13" s="24" t="s">
         <v>24</v>
@@ -1154,7 +1202,7 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="D14" s="23">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="E14" s="24" t="s">
         <v>25</v>
@@ -1162,7 +1210,7 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="D15" s="23">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>26</v>
@@ -1170,7 +1218,7 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="D16" s="23">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="E16" s="24" t="s">
         <v>27</v>
@@ -1178,7 +1226,7 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="D17" s="23">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>28</v>
@@ -1186,1580 +1234,1629 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="D18" s="23">
+        <v>10.0</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="D19" s="23">
         <v>11.0</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1"/>
+      <c r="E19" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
     <row r="22" ht="14.25" customHeight="1"/>
     <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
+      <c r="A25" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="34"/>
       <c r="F25" s="14"/>
     </row>
     <row r="26" ht="25.5" customHeight="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="G26" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="35"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
+      <c r="G26" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="41"/>
     </row>
     <row r="27" ht="25.5" customHeight="1">
-      <c r="A27" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="35"/>
-      <c r="I27" s="40" t="s">
+      <c r="A27" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="35"/>
-      <c r="K27" s="40" t="s">
+      <c r="B27" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="35"/>
-      <c r="M27" s="40" t="s">
+      <c r="C27" s="44"/>
+      <c r="D27" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="35"/>
+      <c r="E27" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="41"/>
+      <c r="I27" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="41"/>
+      <c r="K27" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" s="41"/>
+      <c r="M27" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="N27" s="41"/>
     </row>
     <row r="28" ht="25.5" customHeight="1">
-      <c r="G28" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" s="35"/>
-      <c r="I28" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="J28" s="35"/>
-      <c r="K28" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="35"/>
-      <c r="M28" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="N28" s="35"/>
+      <c r="G28" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="41"/>
+      <c r="I28" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="41"/>
+      <c r="K28" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="L28" s="41"/>
+      <c r="M28" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="N28" s="41"/>
     </row>
     <row r="29" ht="25.5" customHeight="1">
-      <c r="A29" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>45</v>
+      <c r="A29" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>50</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="44" t="s">
-        <v>46</v>
+      <c r="D29" s="50" t="s">
+        <v>51</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="G29" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I29" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="J29" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="K29" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="L29" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="M29" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="N29" s="45" t="s">
-        <v>48</v>
+      <c r="G29" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I29" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="K29" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="L29" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="M29" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="N29" s="51" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" ht="25.5" customHeight="1">
-      <c r="A30" s="46">
+      <c r="A30" s="52">
         <v>1.0</v>
       </c>
-      <c r="B30" s="47" t="s">
-        <v>49</v>
+      <c r="B30" s="53" t="s">
+        <v>54</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="47" t="s">
-        <v>50</v>
+      <c r="D30" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="G30" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J30" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="K30" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L30" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M30" s="48"/>
-      <c r="N30" s="49" t="s">
-        <v>54</v>
+      <c r="G30" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="K30" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L30" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M30" s="54"/>
+      <c r="N30" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="46">
+      <c r="A31" s="52">
         <v>2.0</v>
       </c>
-      <c r="B31" s="47" t="s">
-        <v>55</v>
+      <c r="B31" s="53" t="s">
+        <v>60</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="47" t="s">
-        <v>56</v>
+      <c r="D31" s="53" t="s">
+        <v>61</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="G31" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J31" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="K31" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L31" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M31" s="48"/>
-      <c r="N31" s="49" t="s">
-        <v>54</v>
+      <c r="G31" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L31" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M31" s="54"/>
+      <c r="N31" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="46">
+      <c r="A32" s="52">
         <v>3.0</v>
       </c>
-      <c r="B32" s="47" t="s">
-        <v>57</v>
+      <c r="B32" s="53" t="s">
+        <v>62</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="47" t="s">
-        <v>58</v>
+      <c r="D32" s="53" t="s">
+        <v>63</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="G32" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I32" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J32" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="K32" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L32" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M32" s="48"/>
-      <c r="N32" s="49" t="s">
-        <v>54</v>
+      <c r="G32" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J32" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="K32" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M32" s="54"/>
+      <c r="N32" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="46">
+      <c r="A33" s="52">
         <v>4.0</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="G33" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J33" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="G33" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H33" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J33" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="K33" s="50"/>
+      <c r="K33" s="56"/>
       <c r="L33" s="22"/>
-      <c r="M33" s="50"/>
+      <c r="M33" s="56"/>
       <c r="N33" s="22"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="46">
+      <c r="A34" s="52">
         <v>5.0</v>
       </c>
-      <c r="B34" s="47" t="s">
-        <v>61</v>
+      <c r="B34" s="53" t="s">
+        <v>66</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="47" t="s">
-        <v>62</v>
+      <c r="D34" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="E34" s="5"/>
-      <c r="G34" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H34" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I34" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J34" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="K34" s="50"/>
+      <c r="G34" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H34" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J34" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="K34" s="56"/>
       <c r="L34" s="22"/>
-      <c r="M34" s="50"/>
+      <c r="M34" s="56"/>
       <c r="N34" s="22"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="46">
+      <c r="A35" s="52">
         <v>6.0</v>
       </c>
-      <c r="B35" s="47" t="s">
-        <v>63</v>
+      <c r="B35" s="53" t="s">
+        <v>68</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="47" t="s">
-        <v>64</v>
+      <c r="D35" s="53" t="s">
+        <v>69</v>
       </c>
       <c r="E35" s="5"/>
-      <c r="G35" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H35" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I35" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J35" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="K35" s="50"/>
+      <c r="G35" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J35" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="K35" s="56"/>
       <c r="L35" s="22"/>
-      <c r="M35" s="50"/>
+      <c r="M35" s="56"/>
       <c r="N35" s="22"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="46">
+      <c r="A36" s="52">
         <v>7.0</v>
       </c>
-      <c r="B36" s="47" t="s">
-        <v>65</v>
+      <c r="B36" s="53" t="s">
+        <v>70</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="47" t="s">
-        <v>66</v>
+      <c r="D36" s="53" t="s">
+        <v>71</v>
       </c>
       <c r="E36" s="5"/>
-      <c r="G36" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I36" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J36" s="49" t="s">
-        <v>54</v>
+      <c r="G36" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H36" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="46">
+      <c r="A37" s="52">
         <v>8.0</v>
       </c>
-      <c r="B37" s="47" t="s">
-        <v>67</v>
+      <c r="B37" s="53" t="s">
+        <v>72</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="47" t="s">
-        <v>68</v>
+      <c r="D37" s="53" t="s">
+        <v>73</v>
       </c>
       <c r="E37" s="5"/>
-      <c r="G37" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H37" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I37" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J37" s="49" t="s">
-        <v>54</v>
+      <c r="G37" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="46">
+      <c r="A38" s="52">
         <v>9.0</v>
       </c>
-      <c r="B38" s="47" t="s">
-        <v>69</v>
+      <c r="B38" s="53" t="s">
+        <v>74</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="47" t="s">
-        <v>70</v>
+      <c r="D38" s="53" t="s">
+        <v>75</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="G38" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H38" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I38" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J38" s="49" t="s">
-        <v>54</v>
+      <c r="G38" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H38" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J38" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="46">
+      <c r="A39" s="52">
         <v>10.0</v>
       </c>
-      <c r="B39" s="47" t="s">
-        <v>71</v>
+      <c r="B39" s="53" t="s">
+        <v>76</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="47" t="s">
-        <v>72</v>
+      <c r="D39" s="53" t="s">
+        <v>77</v>
       </c>
       <c r="E39" s="5"/>
-      <c r="G39" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H39" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I39" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J39" s="49" t="s">
-        <v>54</v>
+      <c r="G39" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J39" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="46">
+      <c r="A40" s="52">
         <v>11.0</v>
       </c>
-      <c r="B40" s="47" t="s">
-        <v>73</v>
+      <c r="B40" s="53" t="s">
+        <v>78</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="47" t="s">
-        <v>74</v>
+      <c r="D40" s="53" t="s">
+        <v>79</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="G40" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H40" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I40" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J40" s="49" t="s">
-        <v>54</v>
+      <c r="G40" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J40" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="46">
+      <c r="A41" s="52">
         <v>12.0</v>
       </c>
-      <c r="B41" s="47" t="s">
-        <v>75</v>
+      <c r="B41" s="53" t="s">
+        <v>80</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="47" t="s">
-        <v>76</v>
+      <c r="D41" s="53" t="s">
+        <v>81</v>
       </c>
       <c r="E41" s="5"/>
-      <c r="G41" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H41" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I41" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J41" s="49" t="s">
-        <v>54</v>
+      <c r="G41" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I41" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J41" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1"/>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="G43" s="51" t="s">
+      <c r="G43" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="J43" s="5"/>
+      <c r="K43" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L43" s="5"/>
+      <c r="M43" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N43" s="5"/>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="G44" s="58"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" s="5"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="5"/>
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="G45" s="58"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="5"/>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="G46" s="58"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="5"/>
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="G47" s="58"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="5"/>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="G48" s="58"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="5"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="A51" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" ht="14.25" customHeight="1">
+      <c r="A52" s="35"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="38"/>
+      <c r="G52" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="40"/>
+      <c r="L52" s="40"/>
+      <c r="M52" s="40"/>
+      <c r="N52" s="41"/>
+    </row>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="A53" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="44"/>
+      <c r="D53" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G53" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="H53" s="41"/>
+      <c r="I53" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="J53" s="41"/>
+      <c r="K53" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="L53" s="41"/>
+      <c r="M53" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="N53" s="41"/>
+    </row>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="G54" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="H54" s="41"/>
+      <c r="I54" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="J54" s="41"/>
+      <c r="K54" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="L54" s="41"/>
+      <c r="M54" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="N54" s="41"/>
+    </row>
+    <row r="55" ht="14.25" customHeight="1">
+      <c r="A55" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="G55" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="J55" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="K55" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="L55" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="M55" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="N55" s="51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" ht="14.25" customHeight="1">
+      <c r="A56" s="52">
+        <v>1.0</v>
+      </c>
+      <c r="B56" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="G56" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H56" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I56" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J56" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K56" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L56" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M56" s="54"/>
+      <c r="N56" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" ht="14.25" customHeight="1">
+      <c r="A57" s="52">
+        <v>2.0</v>
+      </c>
+      <c r="B57" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="G57" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H57" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I57" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J57" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K57" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L57" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M57" s="54"/>
+      <c r="N57" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" ht="14.25" customHeight="1">
+      <c r="A58" s="52">
+        <v>3.0</v>
+      </c>
+      <c r="B58" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" s="5"/>
+      <c r="G58" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H58" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I58" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J58" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K58" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L58" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M58" s="54"/>
+      <c r="N58" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" ht="14.25" customHeight="1">
+      <c r="A59" s="52">
+        <v>4.0</v>
+      </c>
+      <c r="B59" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="G59" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H59" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I59" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J59" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K59" s="56"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="56"/>
+      <c r="N59" s="22"/>
+    </row>
+    <row r="60" ht="14.25" customHeight="1">
+      <c r="A60" s="52">
+        <v>5.0</v>
+      </c>
+      <c r="B60" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="G60" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H60" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I60" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J60" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K60" s="56"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="56"/>
+      <c r="N60" s="22"/>
+    </row>
+    <row r="61" ht="14.25" customHeight="1">
+      <c r="A61" s="52">
+        <v>6.0</v>
+      </c>
+      <c r="B61" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="G61" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H61" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I61" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J61" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K61" s="56"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="56"/>
+      <c r="N61" s="22"/>
+    </row>
+    <row r="62" ht="14.25" customHeight="1">
+      <c r="A62" s="52">
+        <v>7.0</v>
+      </c>
+      <c r="B62" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="G62" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H62" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I62" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J62" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" ht="14.25" customHeight="1">
+      <c r="A63" s="52">
+        <v>8.0</v>
+      </c>
+      <c r="B63" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="G63" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H63" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I63" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J63" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25" customHeight="1">
+      <c r="A64" s="52">
+        <v>9.0</v>
+      </c>
+      <c r="B64" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="G64" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H64" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I64" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J64" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="A65" s="52">
+        <v>10.0</v>
+      </c>
+      <c r="B65" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="J43" s="5"/>
-      <c r="K43" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="L43" s="5"/>
-      <c r="M43" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="N43" s="5"/>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="G44" s="52"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="52" t="s">
+      <c r="E65" s="5"/>
+      <c r="G65" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H65" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I65" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J65" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="A66" s="52">
+        <v>11.0</v>
+      </c>
+      <c r="B66" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="J44" s="5"/>
-      <c r="K44" s="52"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="52"/>
-      <c r="N44" s="5"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="G45" s="52"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="52"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="5"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="G46" s="52"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="52"/>
-      <c r="N46" s="5"/>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="G47" s="52"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="52"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="52"/>
-      <c r="N47" s="5"/>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="G48" s="52"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="52"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="5"/>
-    </row>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="25" t="s">
+      <c r="C66" s="5"/>
+      <c r="D66" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="E66" s="5"/>
+      <c r="G66" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H66" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I66" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J66" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" s="52">
+        <v>12.0</v>
+      </c>
+      <c r="B67" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="14"/>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="29"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="32"/>
-      <c r="G52" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="34"/>
-      <c r="M52" s="34"/>
-      <c r="N52" s="35"/>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="38"/>
-      <c r="D53" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E53" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="G53" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="H53" s="35"/>
-      <c r="I53" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="J53" s="35"/>
-      <c r="K53" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="L53" s="35"/>
-      <c r="M53" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="N53" s="35"/>
-    </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="G54" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="H54" s="35"/>
-      <c r="I54" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="J54" s="35"/>
-      <c r="K54" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="L54" s="35"/>
-      <c r="M54" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="N54" s="35"/>
-    </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B55" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E55" s="5"/>
-      <c r="G55" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="H55" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I55" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="J55" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="K55" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="L55" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="M55" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="N55" s="45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="46">
-        <v>1.0</v>
-      </c>
-      <c r="B56" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E56" s="5"/>
-      <c r="G56" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H56" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I56" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J56" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K56" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L56" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M56" s="48"/>
-      <c r="N56" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="46">
-        <v>2.0</v>
-      </c>
-      <c r="B57" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="E57" s="5"/>
-      <c r="G57" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H57" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I57" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J57" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K57" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L57" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M57" s="48"/>
-      <c r="N57" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="46">
-        <v>3.0</v>
-      </c>
-      <c r="B58" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="47" t="s">
+      <c r="C67" s="5"/>
+      <c r="D67" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="G67" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H67" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I67" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J67" s="55" t="s">
         <v>58</v>
-      </c>
-      <c r="E58" s="5"/>
-      <c r="G58" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H58" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I58" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J58" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K58" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L58" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M58" s="48"/>
-      <c r="N58" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="46">
-        <v>4.0</v>
-      </c>
-      <c r="B59" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="E59" s="5"/>
-      <c r="G59" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H59" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I59" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J59" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K59" s="50"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="50"/>
-      <c r="N59" s="22"/>
-    </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="46">
-        <v>5.0</v>
-      </c>
-      <c r="B60" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E60" s="5"/>
-      <c r="G60" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H60" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I60" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J60" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K60" s="50"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="50"/>
-      <c r="N60" s="22"/>
-    </row>
-    <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="46">
-        <v>6.0</v>
-      </c>
-      <c r="B61" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="E61" s="5"/>
-      <c r="G61" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H61" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I61" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J61" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K61" s="50"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="50"/>
-      <c r="N61" s="22"/>
-    </row>
-    <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="46">
-        <v>7.0</v>
-      </c>
-      <c r="B62" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="E62" s="5"/>
-      <c r="G62" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H62" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I62" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J62" s="49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="46">
-        <v>8.0</v>
-      </c>
-      <c r="B63" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="5"/>
-      <c r="G63" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H63" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I63" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J63" s="49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="46">
-        <v>9.0</v>
-      </c>
-      <c r="B64" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" s="5"/>
-      <c r="G64" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H64" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I64" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J64" s="49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="46">
-        <v>10.0</v>
-      </c>
-      <c r="B65" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="E65" s="5"/>
-      <c r="G65" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H65" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I65" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J65" s="49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="46">
-        <v>11.0</v>
-      </c>
-      <c r="B66" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="E66" s="5"/>
-      <c r="G66" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H66" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I66" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J66" s="49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="46">
-        <v>12.0</v>
-      </c>
-      <c r="B67" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="E67" s="5"/>
-      <c r="G67" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H67" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I67" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J67" s="49" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1"/>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="G69" s="51" t="s">
+      <c r="G69" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="H69" s="5"/>
+      <c r="I69" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="J69" s="5"/>
+      <c r="K69" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="L69" s="5"/>
+      <c r="M69" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="N69" s="5"/>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="G70" s="58"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="J70" s="5"/>
+      <c r="K70" s="58"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="58"/>
+      <c r="N70" s="5"/>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="G71" s="58"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="58"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="58"/>
+      <c r="N71" s="5"/>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="G72" s="58"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="58"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="58"/>
+      <c r="N72" s="5"/>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="G73" s="58"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="58"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="58"/>
+      <c r="N73" s="5"/>
+    </row>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="G74" s="58"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="58"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="58"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="58"/>
+      <c r="N74" s="5"/>
+    </row>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1">
+      <c r="A76" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="5"/>
+    </row>
+    <row r="77" ht="14.25" customHeight="1">
+      <c r="A77" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="14"/>
+    </row>
+    <row r="78" ht="14.25" customHeight="1">
+      <c r="A78" s="35"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="38"/>
+      <c r="G78" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H78" s="40"/>
+      <c r="I78" s="40"/>
+      <c r="J78" s="40"/>
+      <c r="K78" s="40"/>
+      <c r="L78" s="40"/>
+      <c r="M78" s="40"/>
+      <c r="N78" s="41"/>
+    </row>
+    <row r="79" ht="14.25" customHeight="1">
+      <c r="A79" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B79" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" s="44"/>
+      <c r="D79" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E79" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="G79" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="H79" s="41"/>
+      <c r="I79" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="J79" s="41"/>
+      <c r="K79" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="L79" s="41"/>
+      <c r="M79" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="N79" s="41"/>
+    </row>
+    <row r="80" ht="14.25" customHeight="1">
+      <c r="G80" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="H80" s="41"/>
+      <c r="I80" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="J80" s="41"/>
+      <c r="K80" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="L80" s="41"/>
+      <c r="M80" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="N80" s="41"/>
+    </row>
+    <row r="81" ht="14.25" customHeight="1">
+      <c r="A81" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" s="5"/>
+      <c r="G81" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H81" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I81" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="J81" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="K81" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="L81" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="M81" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="N81" s="51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" ht="14.25" customHeight="1">
+      <c r="A82" s="52">
+        <v>1.0</v>
+      </c>
+      <c r="B82" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="E82" s="5"/>
+      <c r="G82" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H82" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I82" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J82" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K82" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L82" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M82" s="54"/>
+      <c r="N82" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" ht="14.25" customHeight="1">
+      <c r="A83" s="52">
+        <v>2.0</v>
+      </c>
+      <c r="B83" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="5"/>
+      <c r="D83" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E83" s="5"/>
+      <c r="G83" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H83" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I83" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J83" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K83" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L83" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M83" s="54"/>
+      <c r="N83" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" ht="14.25" customHeight="1">
+      <c r="A84" s="52">
+        <v>3.0</v>
+      </c>
+      <c r="B84" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="5"/>
+      <c r="D84" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="E84" s="5"/>
+      <c r="G84" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H84" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I84" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J84" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K84" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L84" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="M84" s="54"/>
+      <c r="N84" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" ht="14.25" customHeight="1">
+      <c r="A85" s="52">
+        <v>4.0</v>
+      </c>
+      <c r="B85" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="5"/>
+      <c r="G85" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H85" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I85" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J85" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K85" s="56"/>
+      <c r="L85" s="22"/>
+      <c r="M85" s="56"/>
+      <c r="N85" s="22"/>
+    </row>
+    <row r="86" ht="14.25" customHeight="1">
+      <c r="A86" s="52">
+        <v>5.0</v>
+      </c>
+      <c r="B86" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E86" s="5"/>
+      <c r="G86" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H86" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I86" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J86" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="K86" s="56"/>
+      <c r="L86" s="22"/>
+      <c r="M86" s="56"/>
+      <c r="N86" s="22"/>
+    </row>
+    <row r="87" ht="14.25" customHeight="1">
+      <c r="A87" s="52">
+        <v>6.0</v>
+      </c>
+      <c r="B87" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E87" s="5"/>
+      <c r="G87" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H87" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I87" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J87" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="K87" s="56"/>
+      <c r="L87" s="22"/>
+      <c r="M87" s="56"/>
+      <c r="N87" s="22"/>
+    </row>
+    <row r="88" ht="14.25" customHeight="1">
+      <c r="A88" s="52">
+        <v>7.0</v>
+      </c>
+      <c r="B88" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E88" s="5"/>
+      <c r="G88" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H88" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I88" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J88" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" ht="14.25" customHeight="1">
+      <c r="A89" s="52">
+        <v>8.0</v>
+      </c>
+      <c r="B89" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E89" s="5"/>
+      <c r="G89" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H89" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I89" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J89" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" ht="14.25" customHeight="1">
+      <c r="A90" s="52">
+        <v>9.0</v>
+      </c>
+      <c r="B90" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="H69" s="5"/>
-      <c r="I69" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="J69" s="5"/>
-      <c r="K69" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="L69" s="5"/>
-      <c r="M69" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="N69" s="5"/>
-    </row>
-    <row r="70" ht="14.25" customHeight="1">
-      <c r="G70" s="52"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="J70" s="5"/>
-      <c r="K70" s="52"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="52"/>
-      <c r="N70" s="5"/>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="G71" s="52"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="52"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="52"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="52"/>
-      <c r="N71" s="5"/>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="G72" s="52"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="52"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="52"/>
-      <c r="L72" s="5"/>
-      <c r="M72" s="52"/>
-      <c r="N72" s="5"/>
-    </row>
-    <row r="73" ht="14.25" customHeight="1">
-      <c r="G73" s="52"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="52"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="52"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="52"/>
-      <c r="N73" s="5"/>
-    </row>
-    <row r="74" ht="14.25" customHeight="1">
-      <c r="G74" s="52"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="52"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="52"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="52"/>
-      <c r="N74" s="5"/>
-    </row>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B77" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="14"/>
-    </row>
-    <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="29"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="32"/>
-      <c r="G78" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H78" s="34"/>
-      <c r="I78" s="34"/>
-      <c r="J78" s="34"/>
-      <c r="K78" s="34"/>
-      <c r="L78" s="34"/>
-      <c r="M78" s="34"/>
-      <c r="N78" s="35"/>
-    </row>
-    <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B79" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C79" s="38"/>
-      <c r="D79" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E79" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="G79" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="H79" s="35"/>
-      <c r="I79" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="J79" s="35"/>
-      <c r="K79" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="L79" s="35"/>
-      <c r="M79" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="N79" s="35"/>
-    </row>
-    <row r="80" ht="14.25" customHeight="1">
-      <c r="G80" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="H80" s="35"/>
-      <c r="I80" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="J80" s="35"/>
-      <c r="K80" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="L80" s="35"/>
-      <c r="M80" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="N80" s="35"/>
-    </row>
-    <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B81" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="E81" s="5"/>
-      <c r="G81" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="H81" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I81" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="J81" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="K81" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="L81" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="M81" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="N81" s="45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="46">
-        <v>1.0</v>
-      </c>
-      <c r="B82" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E82" s="5"/>
-      <c r="G82" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H82" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I82" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J82" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K82" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L82" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M82" s="48"/>
-      <c r="N82" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="46">
-        <v>2.0</v>
-      </c>
-      <c r="B83" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="E83" s="5"/>
-      <c r="G83" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H83" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I83" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J83" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K83" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L83" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M83" s="48"/>
-      <c r="N83" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="46">
-        <v>3.0</v>
-      </c>
-      <c r="B84" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="E84" s="5"/>
-      <c r="G84" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H84" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I84" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J84" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K84" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="L84" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="M84" s="48"/>
-      <c r="N84" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="46">
-        <v>4.0</v>
-      </c>
-      <c r="B85" s="47" t="s">
+      <c r="E90" s="5"/>
+      <c r="G90" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H90" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I90" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J90" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="E85" s="5"/>
-      <c r="G85" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H85" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I85" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J85" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K85" s="50"/>
-      <c r="L85" s="22"/>
-      <c r="M85" s="50"/>
-      <c r="N85" s="22"/>
-    </row>
-    <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="46">
-        <v>5.0</v>
-      </c>
-      <c r="B86" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E86" s="5"/>
-      <c r="G86" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H86" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I86" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J86" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="K86" s="50"/>
-      <c r="L86" s="22"/>
-      <c r="M86" s="50"/>
-      <c r="N86" s="22"/>
-    </row>
-    <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="46">
-        <v>6.0</v>
-      </c>
-      <c r="B87" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="E87" s="5"/>
-      <c r="G87" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H87" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I87" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J87" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="K87" s="50"/>
-      <c r="L87" s="22"/>
-      <c r="M87" s="50"/>
-      <c r="N87" s="22"/>
-    </row>
-    <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="46">
-        <v>7.0</v>
-      </c>
-      <c r="B88" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="E88" s="5"/>
-      <c r="G88" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H88" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I88" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J88" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="46">
-        <v>8.0</v>
-      </c>
-      <c r="B89" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="E89" s="5"/>
-      <c r="G89" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H89" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I89" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J89" s="49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="46">
-        <v>9.0</v>
-      </c>
-      <c r="B90" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="E90" s="5"/>
-      <c r="G90" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H90" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I90" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J90" s="49" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="46">
+      <c r="A91" s="52">
         <v>10.0</v>
       </c>
-      <c r="B91" s="47" t="s">
-        <v>73</v>
+      <c r="B91" s="53" t="s">
+        <v>78</v>
       </c>
       <c r="C91" s="5"/>
-      <c r="D91" s="47" t="s">
-        <v>74</v>
+      <c r="D91" s="53" t="s">
+        <v>79</v>
       </c>
       <c r="E91" s="5"/>
-      <c r="G91" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H91" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I91" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J91" s="49" t="s">
-        <v>54</v>
+      <c r="G91" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H91" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I91" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J91" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="46">
+      <c r="A92" s="52">
         <v>11.0</v>
       </c>
-      <c r="B92" s="47" t="s">
-        <v>75</v>
+      <c r="B92" s="53" t="s">
+        <v>80</v>
       </c>
       <c r="C92" s="5"/>
-      <c r="D92" s="47" t="s">
-        <v>82</v>
+      <c r="D92" s="53" t="s">
+        <v>88</v>
       </c>
       <c r="E92" s="5"/>
-      <c r="G92" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H92" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="I92" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J92" s="49" t="s">
-        <v>54</v>
+      <c r="G92" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H92" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I92" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J92" s="55" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1"/>
     <row r="94" ht="14.25" customHeight="1"/>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="G95" s="51" t="s">
-        <v>77</v>
+      <c r="G95" s="57" t="s">
+        <v>82</v>
       </c>
       <c r="H95" s="5"/>
-      <c r="I95" s="51" t="s">
-        <v>77</v>
+      <c r="I95" s="57" t="s">
+        <v>82</v>
       </c>
       <c r="J95" s="5"/>
-      <c r="K95" s="51" t="s">
-        <v>77</v>
+      <c r="K95" s="57" t="s">
+        <v>82</v>
       </c>
       <c r="L95" s="5"/>
-      <c r="M95" s="51" t="s">
-        <v>77</v>
+      <c r="M95" s="57" t="s">
+        <v>82</v>
       </c>
       <c r="N95" s="5"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="G96" s="52"/>
+      <c r="G96" s="58"/>
       <c r="H96" s="5"/>
-      <c r="I96" s="52" t="s">
-        <v>86</v>
+      <c r="I96" s="58" t="s">
+        <v>93</v>
       </c>
       <c r="J96" s="5"/>
-      <c r="K96" s="52"/>
+      <c r="K96" s="58"/>
       <c r="L96" s="5"/>
-      <c r="M96" s="52"/>
+      <c r="M96" s="58"/>
       <c r="N96" s="5"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="G97" s="52"/>
+      <c r="G97" s="58"/>
       <c r="H97" s="5"/>
-      <c r="I97" s="52"/>
+      <c r="I97" s="58"/>
       <c r="J97" s="5"/>
-      <c r="K97" s="52"/>
+      <c r="K97" s="58"/>
       <c r="L97" s="5"/>
-      <c r="M97" s="52"/>
+      <c r="M97" s="58"/>
       <c r="N97" s="5"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="G98" s="52"/>
+      <c r="G98" s="58"/>
       <c r="H98" s="5"/>
-      <c r="I98" s="52"/>
+      <c r="I98" s="58"/>
       <c r="J98" s="5"/>
-      <c r="K98" s="52"/>
+      <c r="K98" s="58"/>
       <c r="L98" s="5"/>
-      <c r="M98" s="52"/>
+      <c r="M98" s="58"/>
       <c r="N98" s="5"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="G99" s="52"/>
+      <c r="G99" s="58"/>
       <c r="H99" s="5"/>
-      <c r="I99" s="52"/>
+      <c r="I99" s="58"/>
       <c r="J99" s="5"/>
-      <c r="K99" s="52"/>
+      <c r="K99" s="58"/>
       <c r="L99" s="5"/>
-      <c r="M99" s="52"/>
+      <c r="M99" s="58"/>
       <c r="N99" s="5"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="G100" s="52"/>
+      <c r="G100" s="58"/>
       <c r="H100" s="5"/>
-      <c r="I100" s="52"/>
+      <c r="I100" s="58"/>
       <c r="J100" s="5"/>
-      <c r="K100" s="52"/>
+      <c r="K100" s="58"/>
       <c r="L100" s="5"/>
-      <c r="M100" s="52"/>
+      <c r="M100" s="58"/>
       <c r="N100" s="5"/>
     </row>
     <row r="101" ht="14.25" customHeight="1"/>
@@ -3663,7 +3760,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="182">
+  <mergeCells count="185">
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="I44:J44"/>
@@ -3709,6 +3806,7 @@
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="M27:N27"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:J28"/>
@@ -3747,6 +3845,7 @@
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D50:E50"/>
     <mergeCell ref="G72:H72"/>
     <mergeCell ref="I72:J72"/>
     <mergeCell ref="K72:L72"/>
@@ -3844,8 +3943,9 @@
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B77:E78"/>
     <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:E78"/>
+    <mergeCell ref="D76:E76"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>